<commit_message>
updating spreadsheet to match example
</commit_message>
<xml_diff>
--- a/machineq-keys-indy2018.xlsx
+++ b/machineq-keys-indy2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bencoo01\OneDrive - ARM\Documents\LoRaWANbootcamp-Indi2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ausbla01/scratch/lorawan-bootcamp-indy-2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6DA74C-D85F-4C5A-973B-D410B9658C68}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52586F7D-7A2A-9D45-A5CC-D8F848243D56}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5784" xr2:uid="{E7A6A092-94B2-41AA-A2BC-EE6CE58A5067}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{E7A6A092-94B2-41AA-A2BC-EE6CE58A5067}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>LORA/GenericA.1.0.2_FCC_Rx2-SF12</t>
   </si>
@@ -74,64 +69,43 @@
     <t>DevEUI</t>
   </si>
   <si>
-    <t>AAB3D53E6FFFFB01</t>
-  </si>
-  <si>
-    <t>AAB3D53E6FFFFB02</t>
-  </si>
-  <si>
-    <t>AAB3D53E6FFFFB03</t>
-  </si>
-  <si>
-    <t>21AAFF01</t>
-  </si>
-  <si>
-    <t>21AAFF02</t>
-  </si>
-  <si>
-    <t>21AAFF03</t>
-  </si>
-  <si>
-    <t>21AAFF04</t>
-  </si>
-  <si>
-    <t>BAADC0FFEEBAADC0FFEEBAADC0FFEE01</t>
-  </si>
-  <si>
-    <t>BAADC0FFEEBAADC0FFEEBAADC0FFEE02</t>
-  </si>
-  <si>
-    <t>BAADC0FFEEBAADC0FFEEBAADC0FFEE03</t>
-  </si>
-  <si>
-    <t>BAADC0FFEEBAADC0FFEEBAADC0FFEE04</t>
-  </si>
-  <si>
-    <t>C0FFEEBAADC0FFEEBAADC0FFEEBAAD01</t>
-  </si>
-  <si>
-    <t>C0FFEEBAADC0FFEEBAADC0FFEEBAAD02</t>
-  </si>
-  <si>
-    <t>C0FFEEBAADC0FFEEBAADC0FFEEBAAD03</t>
-  </si>
-  <si>
-    <t>C0FFEEBAADC0FFEEBAADC0FFEEBAAD04</t>
-  </si>
-  <si>
-    <t>AAB3D53E6FFFFB04</t>
-  </si>
-  <si>
-    <t>mbed-ABP-thing1</t>
-  </si>
-  <si>
-    <t>mbed-ABP-thing2</t>
-  </si>
-  <si>
-    <t>mbed-ABP-thing3</t>
-  </si>
-  <si>
-    <t>mbed-ABP-thing4</t>
+    <t>BADDAD01</t>
+  </si>
+  <si>
+    <t>BADDAD02</t>
+  </si>
+  <si>
+    <t>BADDAD03</t>
+  </si>
+  <si>
+    <t>BADDAD04</t>
+  </si>
+  <si>
+    <t>Workshop-Device-01</t>
+  </si>
+  <si>
+    <t>Workshop-Device-02</t>
+  </si>
+  <si>
+    <t>Workshop-Device-03</t>
+  </si>
+  <si>
+    <t>Workshop-Device-04</t>
+  </si>
+  <si>
+    <t>104A15C001FFFF01</t>
+  </si>
+  <si>
+    <t>104A15C001FFFF02</t>
+  </si>
+  <si>
+    <t>104A15C001FFFF03</t>
+  </si>
+  <si>
+    <t>104A15C001FFFF04</t>
+  </si>
+  <si>
+    <t>104A15C001104A15C001104A15C001FF</t>
   </si>
 </sst>
 </file>
@@ -500,24 +474,24 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="50.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="50.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="2"/>
+    <col min="11" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -549,24 +523,24 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -581,21 +555,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>26</v>
@@ -613,24 +587,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>2</v>
@@ -645,24 +619,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>2</v>

</xml_diff>